<commit_message>
created data for top 20 beaches in fl
</commit_message>
<xml_diff>
--- a/CSV/Beaches.xlsx
+++ b/CSV/Beaches.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>https://www.travelinglifestyle.net/best-beaches-florida/</t>
+  </si>
+  <si>
+    <t>Panama City Beach</t>
+  </si>
+  <si>
+    <t>Destin Beach</t>
+  </si>
+  <si>
+    <t>Amelia Island</t>
+  </si>
+  <si>
+    <t>St. Augustine Beach</t>
+  </si>
+  <si>
+    <t>Cocoa Beach</t>
+  </si>
+  <si>
+    <t>Clearwater beach</t>
+  </si>
+  <si>
+    <t>Vero Beach</t>
+  </si>
+  <si>
+    <t>Longboat Key</t>
+  </si>
+  <si>
+    <t>Fort De Soto Park, Tierra Verde</t>
+  </si>
+  <si>
+    <t>Pass-a-Grille Beach, St. Petersburg</t>
+  </si>
+  <si>
+    <t>Siesta Key, Sarasota</t>
+  </si>
+  <si>
+    <t>Blowing Rocks Preserve, Jupiter</t>
+  </si>
+  <si>
+    <t>Jupiter Dog Beach, Jupiter</t>
+  </si>
+  <si>
+    <t>Lighthouse Beach Park, Sanibel Island</t>
+  </si>
+  <si>
+    <t>Captiva Island</t>
+  </si>
+  <si>
+    <t>Bonita Beach Dog Beach, Fort Myers</t>
+  </si>
+  <si>
+    <t>South Beach, Miami</t>
+  </si>
+  <si>
+    <t>Cape Florida State Park, Key Biscayne</t>
+  </si>
+  <si>
+    <t>Smathers Beach</t>
+  </si>
+  <si>
+    <t>Rest Beach</t>
+  </si>
+  <si>
+    <t>Beachd</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -355,17 +424,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>30.176591999999999</v>
+      </c>
+      <c r="C3">
+        <v>-85.805488999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>30.393681000000001</v>
+      </c>
+      <c r="C5">
+        <v>-86.495659000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>30.626570000000001</v>
+      </c>
+      <c r="C7">
+        <v>-81.460853999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>29.85202</v>
+      </c>
+      <c r="C9">
+        <v>-81.267319000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>28.320221</v>
+      </c>
+      <c r="C11">
+        <v>-80.608870999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>27.924440000000001</v>
+      </c>
+      <c r="C13">
+        <v>-82.841003000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>27.63888</v>
+      </c>
+      <c r="C15">
+        <v>-80.389076000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>27.412541999999998</v>
+      </c>
+      <c r="C17">
+        <v>-82.658989000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>27.62509</v>
+      </c>
+      <c r="C19">
+        <v>-82.712639999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>27.695070000000001</v>
+      </c>
+      <c r="C21">
+        <v>-82.735900000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>27.266190000000002</v>
+      </c>
+      <c r="C23">
+        <v>-82.545649999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>26.905529999999999</v>
+      </c>
+      <c r="C25">
+        <v>-80.132080000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>26.934139999999999</v>
+      </c>
+      <c r="C27">
+        <v>-80.099739999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>26.317830000000001</v>
+      </c>
+      <c r="C29">
+        <v>-80.083519999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>26.519850000000002</v>
+      </c>
+      <c r="C31">
+        <v>-82.189903000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>26.43695</v>
+      </c>
+      <c r="C33">
+        <v>-81.92165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>40.688599000000004</v>
+      </c>
+      <c r="C35">
+        <v>-86.762710999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>25.672470000000001</v>
+      </c>
+      <c r="C37">
+        <v>-80.155410000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>29.84056</v>
+      </c>
+      <c r="C39">
+        <v>-81.270579999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>29.262450000000001</v>
+      </c>
+      <c r="C41">
+        <v>-81.156270000000006</v>
       </c>
     </row>
   </sheetData>
@@ -373,5 +676,6 @@
     <hyperlink ref="A1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>